<commit_message>
got it working with the sample folder
</commit_message>
<xml_diff>
--- a/sample_Folder/APP-03009 - 228 US HWY 17 N - Windsor/INSP-0009629_LBP/schedule/2-21 to 2-26 Dewberry Schedule.xlsx
+++ b/sample_Folder/APP-03009 - 228 US HWY 17 N - Windsor/INSP-0009629_LBP/schedule/2-21 to 2-26 Dewberry Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliott\pythonplay\flask\lbp-two\uploads\APP-03009 - 228 US HWY 17 N - Windsor\INSP-0009629_LBP\schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliott\pythonplay\flask\report-big\sample_Folder\APP-03009 - 228 US HWY 17 N - Windsor\INSP-0009629_LBP\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9546B6-D365-4566-B093-07BECFB89833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770263D3-528D-4E02-AE5F-5C95B8CCB8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D2934E6A-7FC9-4785-BB51-4015B81A5E2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{D2934E6A-7FC9-4785-BB51-4015B81A5E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="299">
   <si>
     <t>Florence</t>
   </si>
@@ -866,9 +866,6 @@
   </si>
   <si>
     <t>Ryan</t>
-  </si>
-  <si>
-    <t>Brian</t>
   </si>
   <si>
     <t>Tom</t>
@@ -1715,31 +1712,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB206FD-2DE2-4DBC-BA42-86DA869268C2}">
   <dimension ref="A1:BG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="42.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.6640625" style="1"/>
+    <col min="16" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="3" customFormat="1" ht="14.4">
+    <row r="1" spans="1:59" s="3" customFormat="1" ht="14.5">
       <c r="A1" s="9" t="s">
         <v>259</v>
       </c>
@@ -1831,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="14.4">
+    <row r="3" spans="1:59" ht="14.5">
       <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
@@ -1840,7 +1837,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>56</v>
@@ -1870,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:59" customFormat="1" ht="14.4">
+    <row r="4" spans="1:59" customFormat="1" ht="14.5">
       <c r="A4" s="11" t="s">
         <v>63</v>
       </c>
@@ -1879,7 +1876,7 @@
         <v>64</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>66</v>
@@ -1953,7 +1950,7 @@
       <c r="BF4" s="1"/>
       <c r="BG4" s="1"/>
     </row>
-    <row r="5" spans="1:59" ht="14.4">
+    <row r="5" spans="1:59" ht="14.5">
       <c r="A5" s="11" t="s">
         <v>107</v>
       </c>
@@ -1962,7 +1959,7 @@
         <v>108</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>110</v>
@@ -2036,7 +2033,7 @@
       <c r="BF5"/>
       <c r="BG5"/>
     </row>
-    <row r="6" spans="1:59" ht="14.4">
+    <row r="6" spans="1:59" ht="14.5">
       <c r="A6" s="18" t="s">
         <v>59</v>
       </c>
@@ -2047,7 +2044,7 @@
         <v>60</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>62</v>
@@ -2081,13 +2078,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="27">
+    <row r="7" spans="1:59" ht="26">
       <c r="A7" s="18" t="s">
         <v>202</v>
       </c>
       <c r="B7" s="53"/>
       <c r="C7" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>240</v>
@@ -2120,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="14.4">
+    <row r="8" spans="1:59" ht="14.5">
       <c r="A8" s="18" t="s">
         <v>98</v>
       </c>
@@ -2129,7 +2126,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>101</v>
@@ -2159,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:59" customFormat="1" ht="14.4">
+    <row r="9" spans="1:59" customFormat="1" ht="14.5">
       <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -2191,7 +2188,7 @@
         <v>46</v>
       </c>
       <c r="K9" s="46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L9" s="49">
         <v>44614</v>
@@ -2259,7 +2256,7 @@
         <v>148</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>150</v>
@@ -2289,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="27">
+    <row r="11" spans="1:59" ht="26">
       <c r="A11" s="11" t="s">
         <v>224</v>
       </c>
@@ -2328,21 +2325,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="27">
+    <row r="12" spans="1:59" ht="26">
       <c r="A12" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>240</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F12" s="27" t="s">
         <v>14</v>
@@ -2357,10 +2354,10 @@
         <v>13</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K12" s="40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L12" s="67">
         <v>44614</v>
@@ -2373,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="26.4">
+    <row r="13" spans="1:59" ht="25">
       <c r="A13" s="27" t="s">
         <v>74</v>
       </c>
@@ -2412,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="28.8">
+    <row r="14" spans="1:59" ht="29">
       <c r="A14" s="30" t="s">
         <v>79</v>
       </c>
@@ -2451,12 +2448,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="28.8">
+    <row r="15" spans="1:59" ht="29">
       <c r="A15" s="24" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>245</v>
@@ -2483,7 +2480,7 @@
         <v>97</v>
       </c>
       <c r="K15" s="70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L15" s="73">
         <v>44615</v>
@@ -2521,7 +2518,7 @@
       <c r="AM15"/>
       <c r="AN15"/>
     </row>
-    <row r="16" spans="1:59" ht="14.4">
+    <row r="16" spans="1:59" ht="14.5">
       <c r="A16" s="22" t="s">
         <v>120</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>121</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>123</v>
@@ -2560,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:59" ht="14.4">
+    <row r="17" spans="1:59" ht="14.5">
       <c r="A17" s="22" t="s">
         <v>125</v>
       </c>
@@ -2569,7 +2566,7 @@
         <v>126</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>128</v>
@@ -2599,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:59" customFormat="1" ht="27">
+    <row r="18" spans="1:59" customFormat="1" ht="26">
       <c r="A18" s="22" t="s">
         <v>152</v>
       </c>
@@ -2682,12 +2679,12 @@
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
     </row>
-    <row r="19" spans="1:59" ht="27">
+    <row r="19" spans="1:59" ht="26">
       <c r="A19" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>244</v>
@@ -2714,7 +2711,7 @@
         <v>85</v>
       </c>
       <c r="K19" s="85" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L19" s="67">
         <v>44615</v>
@@ -2727,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:59" ht="27">
+    <row r="20" spans="1:59" ht="26">
       <c r="A20" s="27" t="s">
         <v>206</v>
       </c>
@@ -2736,7 +2733,7 @@
         <v>207</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>209</v>
@@ -2768,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:59" ht="14.4">
+    <row r="21" spans="1:59" ht="14.5">
       <c r="A21" s="27" t="s">
         <v>218</v>
       </c>
@@ -2777,7 +2774,7 @@
         <v>219</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>221</v>
@@ -2809,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:59" customFormat="1" ht="14.4">
+    <row r="22" spans="1:59" customFormat="1" ht="14.5">
       <c r="A22" s="27" t="s">
         <v>229</v>
       </c>
@@ -2818,7 +2815,7 @@
         <v>230</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>232</v>
@@ -2892,18 +2889,18 @@
       <c r="BF22" s="1"/>
       <c r="BG22" s="1"/>
     </row>
-    <row r="23" spans="1:59" ht="14.4">
+    <row r="23" spans="1:59" ht="14.5">
       <c r="A23" s="22" t="s">
         <v>191</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>194</v>
@@ -2924,7 +2921,7 @@
         <v>196</v>
       </c>
       <c r="K23" s="70" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L23" s="88">
         <v>44616</v>
@@ -2937,7 +2934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:59" ht="27">
+    <row r="24" spans="1:59" ht="26">
       <c r="A24" s="22" t="s">
         <v>178</v>
       </c>
@@ -2976,7 +2973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:59" customFormat="1" ht="14.4">
+    <row r="25" spans="1:59" customFormat="1" ht="14.5">
       <c r="A25" s="22" t="s">
         <v>163</v>
       </c>
@@ -2985,7 +2982,7 @@
         <v>164</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>166</v>
@@ -3059,7 +3056,7 @@
       <c r="BF25" s="1"/>
       <c r="BG25" s="1"/>
     </row>
-    <row r="26" spans="1:59" ht="14.4">
+    <row r="26" spans="1:59" ht="14.5">
       <c r="A26" s="22" t="s">
         <v>173</v>
       </c>
@@ -3068,7 +3065,7 @@
         <v>174</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E26" s="24" t="s">
         <v>176</v>
@@ -3103,13 +3100,13 @@
         <v>140</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>141</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>143</v>
@@ -3130,7 +3127,7 @@
         <v>146</v>
       </c>
       <c r="K27" s="85" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L27" s="67">
         <v>44616</v>
@@ -3143,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:59" ht="28.8">
+    <row r="28" spans="1:59" ht="29">
       <c r="A28" s="29" t="s">
         <v>169</v>
       </c>
@@ -3207,7 +3204,7 @@
       <c r="AM28"/>
       <c r="AN28"/>
     </row>
-    <row r="29" spans="1:59" ht="28.8">
+    <row r="29" spans="1:59" ht="29">
       <c r="A29" s="29" t="s">
         <v>187</v>
       </c>
@@ -3246,7 +3243,7 @@
         <v>6</v>
       </c>
       <c r="P29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q29"/>
       <c r="R29"/>
@@ -3273,7 +3270,7 @@
       <c r="AM29"/>
       <c r="AN29"/>
     </row>
-    <row r="30" spans="1:59" ht="28.8">
+    <row r="30" spans="1:59" ht="29">
       <c r="A30" s="32" t="s">
         <v>68</v>
       </c>
@@ -3305,7 +3302,7 @@
         <v>71</v>
       </c>
       <c r="K30" s="61" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L30" s="94">
         <v>44617</v>
@@ -3362,7 +3359,7 @@
       <c r="BF30"/>
       <c r="BG30"/>
     </row>
-    <row r="31" spans="1:59" ht="27">
+    <row r="31" spans="1:59" ht="26">
       <c r="A31" s="18" t="s">
         <v>156</v>
       </c>
@@ -3401,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:59" ht="27">
+    <row r="32" spans="1:59" ht="26">
       <c r="A32" s="18" t="s">
         <v>159</v>
       </c>
@@ -3440,15 +3437,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:59" ht="27">
+    <row r="33" spans="1:59" ht="26">
       <c r="A33" s="22" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="79" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>240</v>
@@ -3472,7 +3469,7 @@
         <v>39</v>
       </c>
       <c r="K33" s="70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L33" s="88">
         <v>44617</v>
@@ -3485,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:59" ht="27">
+    <row r="34" spans="1:59" ht="26">
       <c r="A34" s="22" t="s">
         <v>103</v>
       </c>
@@ -3524,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:59" ht="14.4">
+    <row r="35" spans="1:59" ht="14.5">
       <c r="A35" s="22" t="s">
         <v>113</v>
       </c>
@@ -3533,7 +3530,7 @@
         <v>114</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>116</v>
@@ -3565,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:59" ht="14.4">
+    <row r="36" spans="1:59" ht="14.5">
       <c r="A36" s="22" t="s">
         <v>182</v>
       </c>
@@ -3574,7 +3571,7 @@
         <v>183</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>185</v>
@@ -3604,18 +3601,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:59" ht="14.4">
+    <row r="37" spans="1:59" ht="14.5">
       <c r="A37" s="5" t="s">
         <v>197</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>198</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>200</v>
@@ -3636,7 +3633,7 @@
         <v>201</v>
       </c>
       <c r="K37" s="97" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L37" s="100">
         <v>44618</v>
@@ -3649,7 +3646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:59" ht="28.8">
+    <row r="38" spans="1:59" ht="29">
       <c r="A38" s="5" t="s">
         <v>213</v>
       </c>
@@ -3658,7 +3655,7 @@
         <v>214</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>216</v>
@@ -3690,7 +3687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:59" ht="14.4">
+    <row r="39" spans="1:59" ht="14.5">
       <c r="A39" s="5" t="s">
         <v>234</v>
       </c>
@@ -3699,7 +3696,7 @@
         <v>235</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>237</v>
@@ -3733,7 +3730,7 @@
     </row>
     <row r="40" spans="1:59" ht="25.5" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B40" s="57"/>
       <c r="C40" s="5" t="s">
@@ -3770,7 +3767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:59" ht="14.4">
+    <row r="41" spans="1:59" ht="14.5">
       <c r="A41" s="19" t="s">
         <v>86</v>
       </c>
@@ -3781,7 +3778,7 @@
         <v>87</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>89</v>
@@ -3802,7 +3799,7 @@
         <v>91</v>
       </c>
       <c r="K41" s="58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L41" s="91">
         <v>44618</v>
@@ -3861,19 +3858,19 @@
       <c r="BF41"/>
       <c r="BG41"/>
     </row>
-    <row r="42" spans="1:59" ht="14.4">
+    <row r="42" spans="1:59" ht="14.5">
       <c r="A42" s="38" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B42" s="59"/>
       <c r="C42" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>30</v>
@@ -3885,10 +3882,10 @@
         <v>9</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K42" s="59"/>
       <c r="L42" s="92"/>
@@ -3944,7 +3941,7 @@
       <c r="BF42"/>
       <c r="BG42"/>
     </row>
-    <row r="43" spans="1:59" ht="14.4">
+    <row r="43" spans="1:59" ht="14.5">
       <c r="A43" s="18" t="s">
         <v>130</v>
       </c>
@@ -3953,7 +3950,7 @@
         <v>131</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>133</v>
@@ -4027,7 +4024,7 @@
       <c r="BF43"/>
       <c r="BG43"/>
     </row>
-    <row r="44" spans="1:59" ht="28.8">
+    <row r="44" spans="1:59" ht="29">
       <c r="A44" s="18" t="s">
         <v>135</v>
       </c>
@@ -4036,7 +4033,7 @@
         <v>136</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>138</v>

</xml_diff>